<commit_message>
Convert latest WIP version of p0130r1 to Bikeshed
I had to narrow the performance comparison chart in the Excel document
so that it would not be the widest thing in the page, to avoid messing
with text reflow.
</commit_message>
<xml_diff>
--- a/papers/datatable.xlsx
+++ b/papers/datatable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SG14\Proposals\ComparingVirtualMethods\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\sg14\comparing-virtual-functions\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18110"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="38400" windowHeight="18105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -258,6 +258,9 @@
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-36FA-47C3-8C2A-105ED7A54B61}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -335,6 +338,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-36FA-47C3-8C2A-105ED7A54B61}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -408,6 +416,9 @@
                       <c:h val="8.9178571428571426E-2"/>
                     </c:manualLayout>
                   </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-36FA-47C3-8C2A-105ED7A54B61}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -486,6 +497,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-36FA-47C3-8C2A-105ED7A54B61}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -559,6 +575,9 @@
                       <c:h val="4.9946569178852637E-2"/>
                     </c:manualLayout>
                   </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-36FA-47C3-8C2A-105ED7A54B61}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -636,6 +655,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-36FA-47C3-8C2A-105ED7A54B61}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -709,6 +733,9 @@
                       <c:h val="8.9178571428571426E-2"/>
                     </c:manualLayout>
                   </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-36FA-47C3-8C2A-105ED7A54B61}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -787,6 +814,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-36FA-47C3-8C2A-105ED7A54B61}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -935,7 +967,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1486,8 +1518,8 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>133351</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -1780,13 +1812,13 @@
       <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>0</v>
       </c>
@@ -1794,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>2</v>
       </c>
@@ -1802,7 +1834,7 @@
         <v>0.222715</v>
       </c>
     </row>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>3</v>
       </c>
@@ -1810,7 +1842,7 @@
         <v>0.23644000000000001</v>
       </c>
     </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>4</v>
       </c>
@@ -1818,7 +1850,7 @@
         <v>0.156921</v>
       </c>
     </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>5</v>
       </c>

</xml_diff>